<commit_message>
Fixed filter and template
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_metadata_v3_8_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_metadata_v3_8_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/static/submission_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2818433F-D910-6941-8D22-959ECAA57D03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BE3346-0B28-CA47-868B-C2943FEE94C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15940" xr2:uid="{82938438-56AF-234A-A3B8-D78369EC91CE}"/>
   </bookViews>
@@ -131,7 +131,6 @@
     </font>
     <font>
       <b/>
-      <i/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -199,10 +198,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -568,20 +567,20 @@
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
@@ -596,7 +595,7 @@
       <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="14"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>

</xml_diff>